<commit_message>
Preparatório para entrega da Monografia.
</commit_message>
<xml_diff>
--- a/Cinetico/related_non_functional_resources/Product backlog.xlsx
+++ b/Cinetico/related_non_functional_resources/Product backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Enquanto o usuário realiza um exercício, o sistema irá identificar os pontos de conexão do corpo do usuário e gerar um modelo tridimensional que deverá ser exibido na tela.</t>
   </si>
   <si>
-    <t>Após o usuário fazer um movimento enquanto realiza um exercício, o sistema irá analisar e classificar a ação em Movimento ou Posicionamento.</t>
-  </si>
-  <si>
     <t>Após o usuário fazer um movimento enquanto realiza um exercício, o sistema irá identificar e classificar o tipo de movimento (linear ou angular) e a velocidade de execução.</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Cincluído</t>
+  </si>
+  <si>
+    <t>Após o usuário fazer um movimento enquanto realiza um exercício, o sistema irá analisar e classificar o gesto em em Posicionamento ou Movimentação.</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,35 @@
     <cellStyle name="20% - Ênfase1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="60">
+  <dxfs count="62">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1386,91 +1414,93 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="B3:G17" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" headerRowCellStyle="20% - Ênfase1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="B3:G17" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60" headerRowCellStyle="20% - Ênfase1">
   <autoFilter ref="B3:G17"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="57"/>
-    <tableColumn id="2" name="Nome" dataDxfId="56"/>
-    <tableColumn id="3" name="Importância" dataDxfId="55"/>
-    <tableColumn id="4" name="Estimativa" dataDxfId="54"/>
-    <tableColumn id="5" name="Como Demonstrar" dataDxfId="53"/>
-    <tableColumn id="6" name="Notas" dataDxfId="52"/>
+    <tableColumn id="1" name="ID" dataDxfId="59"/>
+    <tableColumn id="2" name="Nome" dataDxfId="58"/>
+    <tableColumn id="3" name="Importância" dataDxfId="57"/>
+    <tableColumn id="4" name="Estimativa" dataDxfId="56"/>
+    <tableColumn id="5" name="Como Demonstrar" dataDxfId="55"/>
+    <tableColumn id="6" name="Notas" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela6" displayName="Tabela6" ref="B3:K9" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50" tableBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela6" displayName="Tabela6" ref="B3:K9" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52" tableBorderDxfId="51">
   <autoFilter ref="B3:K9"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="Product ID" dataDxfId="48"/>
-    <tableColumn id="2" name="ID Tarefa" dataDxfId="47"/>
-    <tableColumn id="3" name="Tarefa" dataDxfId="46"/>
-    <tableColumn id="4" name="Responsável" dataDxfId="45"/>
-    <tableColumn id="5" name="Estimativa" dataDxfId="44"/>
-    <tableColumn id="6" name="Status" dataDxfId="43"/>
-    <tableColumn id="7" name="Dia 1" dataDxfId="42"/>
-    <tableColumn id="8" name="Dia 2" dataDxfId="41"/>
-    <tableColumn id="9" name="Dia 3" dataDxfId="40"/>
-    <tableColumn id="10" name="Dia 4" dataDxfId="39"/>
+    <tableColumn id="1" name="Product ID" dataDxfId="50"/>
+    <tableColumn id="2" name="ID Tarefa" dataDxfId="49"/>
+    <tableColumn id="3" name="Tarefa" dataDxfId="48"/>
+    <tableColumn id="4" name="Responsável" dataDxfId="47"/>
+    <tableColumn id="5" name="Estimativa" dataDxfId="46"/>
+    <tableColumn id="6" name="Status" dataDxfId="45"/>
+    <tableColumn id="7" name="Dia 1" dataDxfId="44"/>
+    <tableColumn id="8" name="Dia 2" dataDxfId="43"/>
+    <tableColumn id="9" name="Dia 3" dataDxfId="42"/>
+    <tableColumn id="10" name="Dia 4" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="B12:M17" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" tableBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="B12:M17" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
   <autoFilter ref="B12:M17"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Product ID" dataDxfId="35"/>
-    <tableColumn id="2" name="ID Tarefa" dataDxfId="34"/>
-    <tableColumn id="3" name="Tarefa" dataDxfId="33"/>
-    <tableColumn id="4" name="Responsável" dataDxfId="32"/>
-    <tableColumn id="5" name="Estimativa" dataDxfId="31"/>
-    <tableColumn id="6" name="Status" dataDxfId="30"/>
-    <tableColumn id="7" name="Dia 1" dataDxfId="29"/>
-    <tableColumn id="8" name="Dia 2" dataDxfId="28"/>
-    <tableColumn id="9" name="Dia 3" dataDxfId="27"/>
-    <tableColumn id="10" name="Dia 4" dataDxfId="26"/>
-    <tableColumn id="11" name="Dia 5" dataDxfId="25"/>
-    <tableColumn id="12" name="Dia 6" dataDxfId="24"/>
+    <tableColumn id="1" name="Product ID" dataDxfId="37"/>
+    <tableColumn id="2" name="ID Tarefa" dataDxfId="36"/>
+    <tableColumn id="3" name="Tarefa" dataDxfId="35"/>
+    <tableColumn id="4" name="Responsável" dataDxfId="34"/>
+    <tableColumn id="5" name="Estimativa" dataDxfId="33"/>
+    <tableColumn id="6" name="Status" dataDxfId="32"/>
+    <tableColumn id="7" name="Dia 1" dataDxfId="31"/>
+    <tableColumn id="8" name="Dia 2" dataDxfId="30"/>
+    <tableColumn id="9" name="Dia 3" dataDxfId="29"/>
+    <tableColumn id="10" name="Dia 4" dataDxfId="28"/>
+    <tableColumn id="11" name="Dia 5" dataDxfId="27"/>
+    <tableColumn id="12" name="Dia 6" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="B20:J29" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="B20:J29" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" tableBorderDxfId="23">
   <autoFilter ref="B20:J29"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Product ID" dataDxfId="20"/>
-    <tableColumn id="2" name="ID Tarefa" dataDxfId="19"/>
-    <tableColumn id="3" name="Tarefa" dataDxfId="18"/>
-    <tableColumn id="4" name="Responsável" dataDxfId="17"/>
-    <tableColumn id="5" name="Estimativa" dataDxfId="16"/>
-    <tableColumn id="6" name="Status" dataDxfId="15"/>
-    <tableColumn id="7" name="Dia 1" dataDxfId="14"/>
-    <tableColumn id="8" name="Dia 2" dataDxfId="13"/>
-    <tableColumn id="9" name="Dia 3" dataDxfId="12"/>
+    <tableColumn id="1" name="Product ID" dataDxfId="22"/>
+    <tableColumn id="2" name="ID Tarefa" dataDxfId="21"/>
+    <tableColumn id="3" name="Tarefa" dataDxfId="20"/>
+    <tableColumn id="4" name="Responsável" dataDxfId="19"/>
+    <tableColumn id="5" name="Estimativa" dataDxfId="18"/>
+    <tableColumn id="6" name="Status" dataDxfId="17"/>
+    <tableColumn id="7" name="Dia 1" dataDxfId="16"/>
+    <tableColumn id="8" name="Dia 2" dataDxfId="15"/>
+    <tableColumn id="9" name="Dia 3" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="B32:J53" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
-  <autoFilter ref="B32:J53"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Product ID" dataDxfId="8"/>
-    <tableColumn id="2" name="ID Tarefa" dataDxfId="7"/>
-    <tableColumn id="3" name="Tarefa" dataDxfId="6"/>
-    <tableColumn id="4" name="Responsável" dataDxfId="5"/>
-    <tableColumn id="5" name="Estimativa" dataDxfId="4"/>
-    <tableColumn id="6" name="Status" dataDxfId="3"/>
-    <tableColumn id="7" name="Dia 1" dataDxfId="2"/>
-    <tableColumn id="8" name="Dia 2" dataDxfId="1"/>
-    <tableColumn id="9" name="Dia 3" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="B32:L53" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="B32:L53"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Product ID" dataDxfId="10"/>
+    <tableColumn id="2" name="ID Tarefa" dataDxfId="9"/>
+    <tableColumn id="3" name="Tarefa" dataDxfId="8"/>
+    <tableColumn id="4" name="Responsável" dataDxfId="7"/>
+    <tableColumn id="5" name="Estimativa" dataDxfId="6"/>
+    <tableColumn id="6" name="Status" dataDxfId="5"/>
+    <tableColumn id="7" name="Dia 1" dataDxfId="4"/>
+    <tableColumn id="8" name="Dia 2" dataDxfId="3"/>
+    <tableColumn id="9" name="Dia 3" dataDxfId="2"/>
+    <tableColumn id="10" name="Dia 4" dataDxfId="1"/>
+    <tableColumn id="11" name="Dia 5" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1731,7 +1761,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1741,8 +1771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A7" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1814,7 +1844,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="3"/>
@@ -1854,7 +1884,7 @@
         <v>20</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="3"/>
@@ -1874,7 +1904,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="3"/>
@@ -1894,7 +1924,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="3"/>
@@ -1914,7 +1944,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="3"/>
@@ -1934,7 +1964,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="3"/>
@@ -1954,7 +1984,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="3"/>
@@ -1974,7 +2004,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="3"/>
@@ -1994,7 +2024,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="3"/>
@@ -2014,10 +2044,10 @@
         <v>5</v>
       </c>
       <c r="F14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="H14" s="3"/>
     </row>
@@ -2036,7 +2066,7 @@
         <v>10</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="3"/>
@@ -2056,10 +2086,10 @@
         <v>2</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H16" s="3"/>
     </row>
@@ -2078,7 +2108,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="3"/>
@@ -2179,8 +2209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2196,7 +2226,7 @@
   <sheetData>
     <row r="2" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -2211,34 +2241,34 @@
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="D3" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="E3" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>40</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="14" t="s">
-        <v>44</v>
-      </c>
       <c r="K3" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L3" s="1"/>
     </row>
@@ -2250,16 +2280,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F4" s="15">
         <v>1</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H4" s="15">
         <v>80</v>
@@ -2279,16 +2309,16 @@
         <v>2</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F5" s="15">
         <v>1</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H5" s="15">
         <v>100</v>
@@ -2306,16 +2336,16 @@
         <v>3</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F6" s="15">
         <v>1</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H6" s="15">
         <v>100</v>
@@ -2333,16 +2363,16 @@
         <v>4</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F7" s="14">
         <v>1</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H7" s="14">
         <v>100</v>
@@ -2360,16 +2390,16 @@
         <v>5</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" s="15">
         <v>1</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H8" s="15">
         <v>20</v>
@@ -2393,16 +2423,16 @@
         <v>6</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F9" s="15">
         <v>1</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H9" s="16">
         <v>100</v>
@@ -2417,7 +2447,7 @@
     </row>
     <row r="11" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
@@ -2430,40 +2460,40 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="D12" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="E12" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>40</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>3</v>
       </c>
       <c r="G12" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="I12" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="J12" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="J12" s="14" t="s">
-        <v>44</v>
-      </c>
       <c r="K12" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="L12" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="L12" s="20" t="s">
+      <c r="M12" s="20" t="s">
         <v>67</v>
-      </c>
-      <c r="M12" s="20" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="45" x14ac:dyDescent="0.25">
@@ -2474,16 +2504,16 @@
         <v>1</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F13" s="15">
         <v>1</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H13" s="17">
         <v>100</v>
@@ -2502,16 +2532,16 @@
         <v>2</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="17">
+        <v>1</v>
+      </c>
+      <c r="G14" s="17" t="s">
         <v>51</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="17">
-        <v>1</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>52</v>
       </c>
       <c r="H14" s="17">
         <v>100</v>
@@ -2530,16 +2560,16 @@
         <v>3</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F15" s="17">
         <v>2</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H15" s="17">
         <v>50</v>
@@ -2560,16 +2590,16 @@
         <v>4</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F16" s="16">
         <v>2</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H16" s="16">
         <v>10</v>
@@ -2598,16 +2628,16 @@
         <v>5</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F17" s="16">
         <v>1</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H17" s="16">
         <v>100</v>
@@ -2620,7 +2650,7 @@
     </row>
     <row r="19" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
@@ -2631,33 +2661,33 @@
       <c r="I19" s="28"/>
       <c r="J19" s="29"/>
     </row>
-    <row r="20" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="D20" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="E20" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>40</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>3</v>
       </c>
       <c r="G20" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="I20" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I20" s="14" t="s">
+      <c r="J20" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="J20" s="14" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
@@ -2668,19 +2698,23 @@
         <v>1</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F21" s="15">
         <v>10</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H21" s="15"/>
-      <c r="I21" s="14"/>
+        <v>51</v>
+      </c>
+      <c r="H21" s="15">
+        <v>50</v>
+      </c>
+      <c r="I21" s="14">
+        <v>50</v>
+      </c>
       <c r="J21" s="14"/>
     </row>
     <row r="22" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -2691,19 +2725,23 @@
         <v>2</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F22" s="15">
         <v>1</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H22" s="16"/>
-      <c r="I22" s="14"/>
+        <v>51</v>
+      </c>
+      <c r="H22" s="16">
+        <v>50</v>
+      </c>
+      <c r="I22" s="14">
+        <v>50</v>
+      </c>
       <c r="J22" s="14"/>
     </row>
     <row r="23" spans="2:13" ht="45" x14ac:dyDescent="0.25">
@@ -2714,16 +2752,16 @@
         <v>3</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F23" s="15">
         <v>1</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H23" s="15">
         <v>100</v>
@@ -2739,16 +2777,16 @@
         <v>4</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F24" s="15">
         <v>2</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H24" s="15">
         <v>100</v>
@@ -2764,16 +2802,16 @@
         <v>5</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F25" s="15">
         <v>1</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H25" s="15">
         <v>100</v>
@@ -2789,16 +2827,16 @@
         <v>6</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F26" s="15">
         <v>1</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H26" s="15">
         <v>100</v>
@@ -2814,16 +2852,16 @@
         <v>7</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F27" s="15">
         <v>1</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H27" s="16">
         <v>100</v>
@@ -2839,16 +2877,16 @@
         <v>8</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F28" s="15">
         <v>1</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H28" s="15">
         <v>100</v>
@@ -2864,24 +2902,28 @@
         <v>9</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F29" s="15">
         <v>1</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H29" s="16"/>
-      <c r="I29" s="14"/>
+        <v>51</v>
+      </c>
+      <c r="H29" s="16">
+        <v>50</v>
+      </c>
+      <c r="I29" s="14">
+        <v>40</v>
+      </c>
       <c r="J29" s="14"/>
     </row>
     <row r="31" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C31" s="28"/>
       <c r="D31" s="28"/>
@@ -2894,34 +2936,40 @@
     </row>
     <row r="32" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="D32" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="E32" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>40</v>
       </c>
       <c r="F32" s="14" t="s">
         <v>3</v>
       </c>
       <c r="G32" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H32" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H32" s="14" t="s">
+      <c r="I32" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I32" s="14" t="s">
+      <c r="J32" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="J32" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K32" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="L32" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="14">
         <v>4</v>
       </c>
@@ -2929,22 +2977,34 @@
         <v>1</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F33" s="15">
         <v>10</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H33" s="15"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H33" s="15">
+        <v>20</v>
+      </c>
+      <c r="I33" s="14">
+        <v>20</v>
+      </c>
+      <c r="J33" s="14">
+        <v>20</v>
+      </c>
+      <c r="K33" s="20">
+        <v>20</v>
+      </c>
+      <c r="L33" s="20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="14">
         <v>4</v>
       </c>
@@ -2952,22 +3012,24 @@
         <v>2</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F34" s="15">
         <v>1</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H34" s="15"/>
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
-    </row>
-    <row r="35" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+    </row>
+    <row r="35" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B35" s="14">
         <v>5</v>
       </c>
@@ -2975,24 +3037,26 @@
         <v>3</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F35" s="15">
         <v>1</v>
       </c>
       <c r="G35" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H35" s="15">
         <v>100</v>
       </c>
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
-    </row>
-    <row r="36" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+    </row>
+    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="13">
         <v>5</v>
       </c>
@@ -3000,22 +3064,26 @@
         <v>4</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F36" s="15">
         <v>1</v>
       </c>
       <c r="G36" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H36" s="16"/>
+        <v>51</v>
+      </c>
+      <c r="H36" s="16">
+        <v>100</v>
+      </c>
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
-    </row>
-    <row r="37" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+    </row>
+    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="13">
         <v>5</v>
       </c>
@@ -3023,22 +3091,24 @@
         <v>5</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F37" s="15">
         <v>1</v>
       </c>
       <c r="G37" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H37" s="16"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
-    </row>
-    <row r="38" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+    </row>
+    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="22">
         <v>6</v>
       </c>
@@ -3046,22 +3116,26 @@
         <v>6</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F38" s="15">
         <v>1</v>
       </c>
       <c r="G38" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H38" s="16"/>
+        <v>51</v>
+      </c>
+      <c r="H38" s="16">
+        <v>100</v>
+      </c>
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" s="11">
         <v>6</v>
       </c>
@@ -3069,22 +3143,24 @@
         <v>7</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F39" s="15">
         <v>1</v>
       </c>
       <c r="G39" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H39" s="14"/>
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" s="22">
         <v>7</v>
       </c>
@@ -3092,22 +3168,26 @@
         <v>8</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F40" s="15">
         <v>1</v>
       </c>
       <c r="G40" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H40" s="14"/>
+        <v>51</v>
+      </c>
+      <c r="H40" s="14">
+        <v>100</v>
+      </c>
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
-    </row>
-    <row r="41" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+    </row>
+    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="13">
         <v>7</v>
       </c>
@@ -3115,22 +3195,24 @@
         <v>9</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F41" s="15">
         <v>1</v>
       </c>
       <c r="G41" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H41" s="16"/>
       <c r="I41" s="16"/>
       <c r="J41" s="16"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K41" s="20"/>
+      <c r="L41" s="20"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="15">
         <v>8</v>
       </c>
@@ -3138,22 +3220,24 @@
         <v>10</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F42" s="15">
         <v>1</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H42" s="15"/>
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="15">
         <v>8</v>
       </c>
@@ -3161,22 +3245,24 @@
         <v>11</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F43" s="15">
         <v>1</v>
       </c>
       <c r="G43" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H43" s="15"/>
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
-    </row>
-    <row r="44" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K43" s="20"/>
+      <c r="L43" s="20"/>
+    </row>
+    <row r="44" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="14">
         <v>9</v>
       </c>
@@ -3184,24 +3270,26 @@
         <v>12</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F44" s="15">
         <v>1</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H44" s="15">
         <v>100</v>
       </c>
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" s="14">
         <v>9</v>
       </c>
@@ -3209,24 +3297,26 @@
         <v>13</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F45" s="15">
         <v>1</v>
       </c>
       <c r="G45" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H45" s="15">
         <v>100</v>
       </c>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K45" s="20"/>
+      <c r="L45" s="20"/>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" s="15">
         <v>9</v>
       </c>
@@ -3234,22 +3324,30 @@
         <v>14</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F46" s="15">
         <v>2</v>
       </c>
       <c r="G46" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H46" s="15"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-    </row>
-    <row r="47" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H46" s="15">
+        <v>50</v>
+      </c>
+      <c r="I46" s="14">
+        <v>40</v>
+      </c>
+      <c r="J46" s="14">
+        <v>10</v>
+      </c>
+      <c r="K46" s="20"/>
+      <c r="L46" s="20"/>
+    </row>
+    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="14">
         <v>9</v>
       </c>
@@ -3257,22 +3355,24 @@
         <v>15</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F47" s="15">
         <v>1</v>
       </c>
       <c r="G47" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H47" s="16"/>
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K47" s="20"/>
+      <c r="L47" s="20"/>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" s="14">
         <v>10</v>
       </c>
@@ -3280,22 +3380,26 @@
         <v>16</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F48" s="15">
         <v>1</v>
       </c>
       <c r="G48" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H48" s="15"/>
+        <v>51</v>
+      </c>
+      <c r="H48" s="15">
+        <v>100</v>
+      </c>
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K48" s="20"/>
+      <c r="L48" s="20"/>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" s="14">
         <v>10</v>
       </c>
@@ -3303,22 +3407,24 @@
         <v>17</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F49" s="15">
         <v>1</v>
       </c>
       <c r="G49" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H49" s="15"/>
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
-    </row>
-    <row r="50" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K49" s="20"/>
+      <c r="L49" s="20"/>
+    </row>
+    <row r="50" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B50" s="14">
         <v>12</v>
       </c>
@@ -3326,24 +3432,26 @@
         <v>18</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F50" s="15">
         <v>1</v>
       </c>
       <c r="G50" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H50" s="15">
         <v>100</v>
       </c>
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" s="15">
         <v>12</v>
       </c>
@@ -3351,22 +3459,24 @@
         <v>19</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F51" s="15">
         <v>10</v>
       </c>
       <c r="G51" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H51" s="15"/>
       <c r="I51" s="14"/>
       <c r="J51" s="14"/>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K51" s="20"/>
+      <c r="L51" s="20"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" s="15">
         <v>12</v>
       </c>
@@ -3374,22 +3484,24 @@
         <v>20</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F52" s="15">
         <v>2</v>
       </c>
       <c r="G52" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H52" s="15"/>
       <c r="I52" s="14"/>
       <c r="J52" s="14"/>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K52" s="20"/>
+      <c r="L52" s="20"/>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" s="14">
         <v>12</v>
       </c>
@@ -3397,20 +3509,22 @@
         <v>21</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F53" s="15">
         <v>2</v>
       </c>
       <c r="G53" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H53" s="15"/>
       <c r="I53" s="14"/>
       <c r="J53" s="14"/>
+      <c r="K53" s="20"/>
+      <c r="L53" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>